<commit_message>
add earnings in excel and json
</commit_message>
<xml_diff>
--- a/bestPlayers.xlsx
+++ b/bestPlayers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neo Dossier Alexis\Web Projects\BrawlhallaBestCountryPlayersRanksBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F72DE92-803F-4F32-B53E-E0FCE709770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF04548-AE51-4A49-A6B3-4FF0F4F828FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Xefitra</t>
   </si>
   <si>
-    <t>Zapapy</t>
-  </si>
-  <si>
     <t>Zoraner</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>Mahé</t>
   </si>
   <si>
-    <t>Ecran (Hz)</t>
-  </si>
-  <si>
     <t>Saiyajin</t>
   </si>
   <si>
@@ -280,13 +274,34 @@
   </si>
   <si>
     <t>Shadra</t>
+  </si>
+  <si>
+    <t>Stayn</t>
+  </si>
+  <si>
+    <t>Jacques</t>
+  </si>
+  <si>
+    <t>Lazar Spinola</t>
+  </si>
+  <si>
+    <t>Earnings</t>
+  </si>
+  <si>
+    <t>ZapapY</t>
+  </si>
+  <si>
+    <t>Screen (Hz)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,14 +313,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -348,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,15 +416,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}" name="France" displayName="France" ref="A1:C83" totalsRowShown="0">
-  <autoFilter ref="A1:C83" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C83">
-    <sortCondition ref="A1:A83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}" name="France" displayName="France" ref="A1:D86" totalsRowShown="0">
+  <autoFilter ref="A1:D86" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D86">
+    <sortCondition ref="A1:A86"/>
   </sortState>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D71A5C60-C9CB-4021-B21A-999D15C973E7}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{72C08557-87CE-4BA1-96A4-01F97269FA83}" name="Brawlhalla ID" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{622C6FC7-BEA6-4997-8416-1FB85B56A52A}" name="Ecran (Hz)" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{622C6FC7-BEA6-4997-8416-1FB85B56A52A}" name="Earnings" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{B9C81D88-2D1B-4EC0-A9DA-84B0DFA25082}" name="Screen (Hz)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -686,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +710,7 @@
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,192 +718,236 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>2123759</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>62672086</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>18711253</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>10336731</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>2643269</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>4281946</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>41316701</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>6319950</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="2">
         <v>25254254</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
         <v>158608</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>9238331</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2">
         <v>4608774</v>
       </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="2">
         <v>12939784</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2">
         <v>5424846</v>
       </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2">
         <v>1367587</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="4">
+        <v>3377</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="2">
         <v>4303475</v>
       </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="4">
+        <v>4150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2">
         <v>1279448</v>
       </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="2">
         <v>19800966</v>
       </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="2">
         <v>4563514</v>
       </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="2">
         <v>4708483</v>
       </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -903,551 +955,710 @@
         <v>3540146</v>
       </c>
       <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
         <v>360</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="2">
         <v>10439301</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2">
         <v>8615459</v>
       </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="2">
         <v>27433024</v>
       </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B26" s="2">
         <v>9099776</v>
       </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" s="2">
         <v>23595564</v>
       </c>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="2">
         <v>1819594</v>
       </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1105093</v>
+      </c>
+      <c r="C30" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="2">
         <v>30830337</v>
       </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="2">
         <v>45168975</v>
       </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="2">
-        <v>3184429</v>
-      </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="4">
+        <v>3000</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" s="2">
-        <v>32891165</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>3184429</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="B34" s="2">
-        <v>200122</v>
-      </c>
-      <c r="C34" s="2"/>
+        <v>32891165</v>
+      </c>
+      <c r="C34" s="4">
+        <v>150</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="2">
-        <v>9558549</v>
-      </c>
-      <c r="C35" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>23</v>
+      <c r="A36" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B36" s="2">
-        <v>628502</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>200122</v>
+      </c>
+      <c r="C36" s="4">
+        <v>25220</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2">
+        <v>9558549</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="2">
+        <v>628502</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2">
         <v>2875216</v>
       </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="2">
-        <v>63706748</v>
-      </c>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="2">
-        <v>9542361</v>
-      </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="2">
-        <v>33132832</v>
-      </c>
-      <c r="C40" s="2"/>
+        <v>63706748</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>26</v>
+      <c r="A41" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B41" s="2">
-        <v>37962038</v>
-      </c>
-      <c r="C41" s="2"/>
+        <v>9542361</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B42" s="2">
-        <v>588314</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>33132832</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B43" s="2">
-        <v>10080900</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>37962038</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B44" s="2">
-        <v>1240977</v>
-      </c>
-      <c r="C44" s="2"/>
+        <v>588314</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B45" s="2">
-        <v>6328368</v>
-      </c>
-      <c r="C45" s="2"/>
+        <v>10080900</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="B46" s="2">
-        <v>2118780</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>1240977</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="B47" s="2">
-        <v>63730170</v>
-      </c>
-      <c r="C47" s="2"/>
+        <v>6328368</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B48" s="2">
-        <v>24778112</v>
-      </c>
-      <c r="C48" s="2"/>
+        <v>2118780</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B49" s="2">
-        <v>1862459</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>63730170</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B50" s="2">
-        <v>7555072</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>24778112</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="A51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1862459</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="2">
+        <v>7555072</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B54" s="2">
         <v>9633608</v>
       </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="C54" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B55" s="2">
         <v>2869327</v>
       </c>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="C55" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B56" s="2">
         <v>72329317</v>
       </c>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="C56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" s="2">
+      <c r="B57" s="2"/>
+      <c r="C57" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="2">
         <v>4138490</v>
       </c>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57" s="2">
-        <v>337254</v>
-      </c>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="C58" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>7970886</v>
-      </c>
-      <c r="C59" s="2"/>
+        <v>337254</v>
+      </c>
+      <c r="C59" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" s="2">
-        <v>32417896</v>
-      </c>
-      <c r="C60" s="2"/>
+      <c r="A60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B61" s="2">
-        <v>70129836</v>
-      </c>
-      <c r="C61" s="2"/>
+        <v>7970886</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B62" s="2">
-        <v>4454684</v>
-      </c>
-      <c r="C62" s="2"/>
+        <v>32417896</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B63" s="2">
-        <v>7470522</v>
-      </c>
-      <c r="C63" s="2"/>
+        <v>70129836</v>
+      </c>
+      <c r="C63" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B64" s="2">
+        <v>4454684</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="2">
+        <v>7470522</v>
+      </c>
+      <c r="C65" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" s="2">
         <v>7159263</v>
       </c>
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="C66" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B67" s="2">
         <v>61841362</v>
       </c>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="C67" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B68" s="2">
         <v>5805481</v>
       </c>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="2">
+      <c r="C68" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2">
         <v>25296520</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C69" s="4">
+        <v>3825</v>
+      </c>
+      <c r="D69" s="2">
         <v>390</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B68" s="2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="2">
         <v>3570888</v>
       </c>
-      <c r="C68" s="2"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B69" s="2">
+      <c r="C70" s="4">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="2">
+        <v>481854</v>
+      </c>
+      <c r="C71" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72" s="2">
         <v>1627540</v>
       </c>
-      <c r="C69" s="2"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="C72" s="4">
+        <v>3672</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B73" s="2">
         <v>39768578</v>
       </c>
-      <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="C73" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B74" s="2">
         <v>2412539</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C74" s="4">
+        <v>26180</v>
+      </c>
+      <c r="D74" s="2">
         <v>360</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B75" s="2">
         <v>338489</v>
       </c>
-      <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="C75" s="4">
+        <v>6105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B76" s="2">
         <v>8830089</v>
       </c>
-      <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="C76" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B77" s="2">
         <v>3252577</v>
       </c>
-      <c r="C74" s="2"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="C77" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="B78" s="2"/>
+      <c r="C78" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B77" s="2">
+      <c r="B79" s="2"/>
+      <c r="C79" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="2">
         <v>7808660</v>
       </c>
-      <c r="C77" s="2"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B78" s="2">
-        <v>4444124</v>
-      </c>
-      <c r="C78" s="2"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B79" s="2">
-        <v>5006383</v>
-      </c>
-      <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B80" s="2">
-        <v>56869252</v>
-      </c>
-      <c r="C80" s="2"/>
+      <c r="C80" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B81" s="2">
-        <v>1257608</v>
-      </c>
-      <c r="C81" s="2"/>
+        <v>4444124</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="B82" s="2">
+        <v>5006383</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B83" s="2">
+        <v>56869252</v>
+      </c>
+      <c r="C83" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="2">
+        <v>1257608</v>
+      </c>
+      <c r="C84" s="4">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="2">
         <v>9757291</v>
       </c>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B83" s="2">
+      <c r="C85" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" s="2">
         <v>67424649</v>
       </c>
-      <c r="C83" s="2"/>
+      <c r="C86" s="4">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update excel / change to 3 json updates
</commit_message>
<xml_diff>
--- a/bestPlayers.xlsx
+++ b/bestPlayers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neo Dossier Alexis\Web Projects\BrawlhallaBestCountryPlayersRanksBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B940368B-5676-4B9E-8497-A4DAE6C35A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46D7077-DFA8-4252-80F4-0A39B013A661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Fezaru80</t>
   </si>
   <si>
-    <t>Fzm</t>
-  </si>
-  <si>
     <t>IIceJotaro</t>
   </si>
   <si>
@@ -162,12 +159,6 @@
     <t>Urbador</t>
   </si>
   <si>
-    <t>Vexxuxe</t>
-  </si>
-  <si>
-    <t>Vixa</t>
-  </si>
-  <si>
     <t>VP</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
     <t>Saiyajin</t>
   </si>
   <si>
-    <t>B.A.T | Zoro</t>
-  </si>
-  <si>
     <t>Clap</t>
   </si>
   <si>
@@ -222,9 +210,6 @@
     <t>Spectre.</t>
   </si>
   <si>
-    <t>SanMax™</t>
-  </si>
-  <si>
     <t>Romanraa</t>
   </si>
   <si>
@@ -234,9 +219,6 @@
     <t>OxVenn</t>
   </si>
   <si>
-    <t>Saphir£</t>
-  </si>
-  <si>
     <t>SpyroX</t>
   </si>
   <si>
@@ -252,9 +234,6 @@
     <t>Machèèèèté</t>
   </si>
   <si>
-    <t>ExodiiiiiiiA</t>
-  </si>
-  <si>
     <t>zBlackneight</t>
   </si>
   <si>
@@ -298,6 +277,75 @@
   </si>
   <si>
     <t>Yann_X</t>
+  </si>
+  <si>
+    <t>ExodiA</t>
+  </si>
+  <si>
+    <t>Saphir?</t>
+  </si>
+  <si>
+    <t>Crunchy</t>
+  </si>
+  <si>
+    <t>Qan</t>
+  </si>
+  <si>
+    <t>VorTex_Alexis</t>
+  </si>
+  <si>
+    <t>Mehdou</t>
+  </si>
+  <si>
+    <t>Yamaha</t>
+  </si>
+  <si>
+    <t>cLuK</t>
+  </si>
+  <si>
+    <t>ASX_BH</t>
+  </si>
+  <si>
+    <t>Bouss</t>
+  </si>
+  <si>
+    <t>Xorldz</t>
+  </si>
+  <si>
+    <t>Cana</t>
+  </si>
+  <si>
+    <t>Phobie</t>
+  </si>
+  <si>
+    <t>B.A.T | ZORO</t>
+  </si>
+  <si>
+    <t>SanMax</t>
+  </si>
+  <si>
+    <t>Meydey</t>
+  </si>
+  <si>
+    <t>Vexuxe</t>
+  </si>
+  <si>
+    <t>Azatsu</t>
+  </si>
+  <si>
+    <t>BanLePoulpe</t>
+  </si>
+  <si>
+    <t>MT | RTZ</t>
+  </si>
+  <si>
+    <t>Sorkez</t>
+  </si>
+  <si>
+    <t>FzM</t>
+  </si>
+  <si>
+    <t>SnaKe</t>
   </si>
 </sst>
 </file>
@@ -307,7 +355,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,13 +365,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
@@ -363,14 +404,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -436,10 +475,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}" name="France" displayName="France" ref="A1:D88" totalsRowShown="0">
-  <autoFilter ref="A1:D88" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D88">
-    <sortCondition ref="A1:A88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}" name="France" displayName="France" ref="A1:D104" totalsRowShown="0">
+  <autoFilter ref="A1:D104" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D104">
+    <sortCondition ref="A1:A104"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D71A5C60-C9CB-4021-B21A-999D15C973E7}" name="Name" dataDxfId="2"/>
@@ -714,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,15 +777,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -758,10 +797,10 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -844,33 +883,33 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
+      <c r="A10" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B10" s="2">
+        <v>29733011</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2748864</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="2">
         <v>25254254</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>158608</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>9238331</v>
       </c>
       <c r="C12" s="4">
         <v>0</v>
@@ -878,21 +917,21 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2">
-        <v>4608774</v>
+        <v>6406021</v>
       </c>
       <c r="C13" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>56</v>
+      <c r="A14" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B14" s="2">
-        <v>12939784</v>
+        <v>158608</v>
       </c>
       <c r="C14" s="4">
         <v>0</v>
@@ -900,10 +939,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="B15" s="2">
-        <v>5424846</v>
+        <v>7175314</v>
       </c>
       <c r="C15" s="4">
         <v>0</v>
@@ -911,43 +950,43 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2">
-        <v>1367587</v>
+        <v>4455324</v>
       </c>
       <c r="C16" s="4">
-        <v>3377</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="2">
-        <v>48772510</v>
+        <v>9238331</v>
       </c>
       <c r="C17" s="4">
-        <v>4150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2">
-        <v>1279448</v>
+        <v>4608774</v>
       </c>
       <c r="C18" s="4">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B19" s="2">
-        <v>19800966</v>
+        <v>23477768</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -955,10 +994,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2">
-        <v>4563514</v>
+        <v>12939784</v>
       </c>
       <c r="C20" s="4">
         <v>0</v>
@@ -966,10 +1005,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2">
-        <v>4708483</v>
+        <v>5424846</v>
       </c>
       <c r="C21" s="4">
         <v>0</v>
@@ -977,60 +1016,54 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="B22" s="2">
-        <v>3540146</v>
+        <v>9403791</v>
       </c>
       <c r="C22" s="4">
         <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2">
-        <v>25116293</v>
+        <v>1367587</v>
       </c>
       <c r="C23" s="4">
-        <v>0</v>
+        <v>3377</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2">
-        <v>10439301</v>
+        <v>48772510</v>
       </c>
       <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>60</v>
+        <v>4150</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2">
-        <v>8615459</v>
+        <v>1279448</v>
       </c>
       <c r="C25" s="4">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B26" s="2">
-        <v>27433024</v>
+        <v>19800966</v>
       </c>
       <c r="C26" s="4">
         <v>0</v>
@@ -1038,10 +1071,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2">
-        <v>9099776</v>
+        <v>4563514</v>
       </c>
       <c r="C27" s="4">
         <v>0</v>
@@ -1049,10 +1082,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="B28" s="2">
-        <v>23595564</v>
+        <v>4708483</v>
       </c>
       <c r="C28" s="4">
         <v>0</v>
@@ -1060,41 +1093,49 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B29" s="2">
-        <v>1819594</v>
+        <v>3540146</v>
       </c>
       <c r="C29" s="4">
         <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>360</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="B30" s="2">
+        <v>25116293</v>
+      </c>
       <c r="C30" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B31" s="2">
-        <v>1105093</v>
+        <v>10439301</v>
       </c>
       <c r="C31" s="4">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="B32" s="2">
-        <v>30830337</v>
+        <v>8615459</v>
       </c>
       <c r="C32" s="4">
         <v>0</v>
@@ -1102,21 +1143,21 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B33" s="2">
-        <v>45168975</v>
+        <v>27433024</v>
       </c>
       <c r="C33" s="4">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B34" s="2">
-        <v>3184429</v>
+        <v>9099776</v>
       </c>
       <c r="C34" s="4">
         <v>0</v>
@@ -1124,52 +1165,52 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B35" s="2">
-        <v>5270270</v>
+        <v>23595564</v>
       </c>
       <c r="C35" s="4">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1819594</v>
+      </c>
       <c r="C36" s="4">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="2">
-        <v>200122</v>
-      </c>
+      <c r="A37" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="2"/>
       <c r="C37" s="4">
-        <v>25220</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B38" s="2">
-        <v>9558549</v>
+        <v>1105093</v>
       </c>
       <c r="C38" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>22</v>
+      <c r="A39" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B39" s="2">
-        <v>628502</v>
+        <v>30830337</v>
       </c>
       <c r="C39" s="4">
         <v>0</v>
@@ -1177,65 +1218,63 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B40" s="2">
-        <v>2875216</v>
+        <v>45168975</v>
       </c>
       <c r="C40" s="4">
-        <v>80</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B41" s="2">
-        <v>63706748</v>
+        <v>3184429</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>57</v>
+      <c r="A42" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B42" s="2">
-        <v>9542361</v>
+        <v>5270270</v>
       </c>
       <c r="C42" s="4">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="2">
-        <v>33132832</v>
-      </c>
+      <c r="A43" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="2"/>
       <c r="C43" s="4">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B44" s="2">
-        <v>37962038</v>
+        <v>200122</v>
       </c>
       <c r="C44" s="4">
-        <v>0</v>
+        <v>25220</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B45" s="2">
-        <v>588314</v>
+        <v>9558549</v>
       </c>
       <c r="C45" s="4">
         <v>0</v>
@@ -1243,10 +1282,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B46" s="2">
-        <v>7677560</v>
+        <v>628502</v>
       </c>
       <c r="C46" s="4">
         <v>0</v>
@@ -1254,21 +1293,21 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2">
-        <v>1240977</v>
+        <v>2875216</v>
       </c>
       <c r="C47" s="4">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="B48" s="2">
-        <v>6328368</v>
+        <v>55716814</v>
       </c>
       <c r="C48" s="4">
         <v>0</v>
@@ -1276,10 +1315,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B49" s="2">
-        <v>10080900</v>
+        <v>63706748</v>
       </c>
       <c r="C49" s="4">
         <v>0</v>
@@ -1287,10 +1326,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" s="2">
-        <v>2118780</v>
+        <v>63747925</v>
       </c>
       <c r="C50" s="4">
         <v>0</v>
@@ -1298,10 +1337,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B51" s="2">
-        <v>63730170</v>
+        <v>9542361</v>
       </c>
       <c r="C51" s="4">
         <v>0</v>
@@ -1309,10 +1348,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="B52" s="2">
-        <v>24778112</v>
+        <v>27400066</v>
       </c>
       <c r="C52" s="4">
         <v>0</v>
@@ -1320,10 +1359,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="B53" s="2">
-        <v>1862459</v>
+        <v>33132832</v>
       </c>
       <c r="C53" s="4">
         <v>0</v>
@@ -1331,72 +1370,76 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="B54" s="2">
-        <v>7555072</v>
+        <v>37962038</v>
       </c>
       <c r="C54" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B55" s="2"/>
+      <c r="A55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="2">
+        <v>588314</v>
+      </c>
       <c r="C55" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="B56" s="2">
-        <v>9633608</v>
+        <v>7677560</v>
       </c>
       <c r="C56" s="4">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B57" s="2">
-        <v>2869327</v>
+        <v>1240977</v>
       </c>
       <c r="C57" s="4">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>33</v>
+      <c r="A58" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B58" s="2">
-        <v>72329317</v>
+        <v>6328368</v>
       </c>
       <c r="C58" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B59" s="2"/>
+      <c r="A59" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="2">
+        <v>10080900</v>
+      </c>
       <c r="C59" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>4138490</v>
+        <v>2118780</v>
       </c>
       <c r="C60" s="4">
         <v>0</v>
@@ -1404,30 +1447,32 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B61" s="2">
-        <v>337254</v>
+        <v>63730170</v>
       </c>
       <c r="C61" s="4">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B62" s="2"/>
+      <c r="A62" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="2">
+        <v>6246821</v>
+      </c>
       <c r="C62" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B63" s="2">
-        <v>7970886</v>
+        <v>24778112</v>
       </c>
       <c r="C63" s="4">
         <v>0</v>
@@ -1435,285 +1480,458 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B64" s="2">
+        <v>1862459</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="2">
+        <v>7555072</v>
+      </c>
+      <c r="C65" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" s="2">
+        <v>4101132</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" s="2">
+        <v>8490982</v>
+      </c>
+      <c r="C67" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="2">
+        <v>9633608</v>
+      </c>
+      <c r="C68" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2869327</v>
+      </c>
+      <c r="C69" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" s="2">
+        <v>72329317</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" s="2">
+        <v>6193054</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" s="2">
+        <v>4138490</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" s="2">
+        <v>337254</v>
+      </c>
+      <c r="C73" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75" s="2">
+        <v>7970886</v>
+      </c>
+      <c r="C75" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B76" s="2">
         <v>32417896</v>
       </c>
-      <c r="C64" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="C76" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="2">
+        <v>70129836</v>
+      </c>
+      <c r="C77" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" s="2">
+        <v>4454684</v>
+      </c>
+      <c r="C78" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" s="2">
+        <v>7470522</v>
+      </c>
+      <c r="C79" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80" s="2">
+        <v>7159263</v>
+      </c>
+      <c r="C80" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B81" s="2">
+        <v>61841362</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="2">
+        <v>5805481</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B83" s="2">
+        <v>6301236</v>
+      </c>
+      <c r="C83" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" s="2">
+        <v>6414474</v>
+      </c>
+      <c r="C84" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B85" s="2">
+        <v>25296520</v>
+      </c>
+      <c r="C85" s="4">
+        <v>3825</v>
+      </c>
+      <c r="D85" s="2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B86" s="2">
+        <v>3570888</v>
+      </c>
+      <c r="C86" s="4">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B87" s="2">
+        <v>481854</v>
+      </c>
+      <c r="C87" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B88" s="2">
+        <v>1627540</v>
+      </c>
+      <c r="C88" s="4">
+        <v>3672</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" s="2">
+        <v>39768578</v>
+      </c>
+      <c r="C89" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B90" s="2">
+        <v>2412539</v>
+      </c>
+      <c r="C90" s="4">
+        <v>26180</v>
+      </c>
+      <c r="D90" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B91" s="2">
+        <v>338489</v>
+      </c>
+      <c r="C91" s="4">
+        <v>6105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B92" s="2">
+        <v>8830089</v>
+      </c>
+      <c r="C92" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B93" s="2">
+        <v>3252577</v>
+      </c>
+      <c r="C93" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94" s="2">
+        <v>807434</v>
+      </c>
+      <c r="C94" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B95" s="2">
+        <v>7808660</v>
+      </c>
+      <c r="C95" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B96" s="2">
+        <v>4444124</v>
+      </c>
+      <c r="C96" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B97" s="2">
+        <v>5006383</v>
+      </c>
+      <c r="C97" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B98" s="2">
+        <v>1569376</v>
+      </c>
+      <c r="C98" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B99" s="2">
+        <v>56869252</v>
+      </c>
+      <c r="C99" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B100" s="2">
+        <v>5034931</v>
+      </c>
+      <c r="C100" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B101" s="2">
+        <v>1823973</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B102" s="2">
+        <v>1257608</v>
+      </c>
+      <c r="C102" s="4">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="2">
-        <v>70129836</v>
-      </c>
-      <c r="C65" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B66" s="2">
-        <v>4454684</v>
-      </c>
-      <c r="C66" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B67" s="2">
-        <v>7470522</v>
-      </c>
-      <c r="C67" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B68" s="2">
-        <v>7159263</v>
-      </c>
-      <c r="C68" s="4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B69" s="2">
-        <v>61841362</v>
-      </c>
-      <c r="C69" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B70" s="2">
-        <v>5805481</v>
-      </c>
-      <c r="C70" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B71" s="2">
-        <v>25296520</v>
-      </c>
-      <c r="C71" s="4">
-        <v>3825</v>
-      </c>
-      <c r="D71" s="2">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="2">
-        <v>3570888</v>
-      </c>
-      <c r="C72" s="4">
-        <v>1720</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" s="2">
-        <v>481854</v>
-      </c>
-      <c r="C73" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74" s="2">
-        <v>1627540</v>
-      </c>
-      <c r="C74" s="4">
-        <v>3672</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B75" s="2">
-        <v>39768578</v>
-      </c>
-      <c r="C75" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B76" s="2">
-        <v>2412539</v>
-      </c>
-      <c r="C76" s="4">
-        <v>26180</v>
-      </c>
-      <c r="D76" s="2">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="2">
-        <v>338489</v>
-      </c>
-      <c r="C77" s="4">
-        <v>6105</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B78" s="2">
-        <v>8830089</v>
-      </c>
-      <c r="C78" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B79" s="2">
-        <v>3252577</v>
-      </c>
-      <c r="C79" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="B103" s="2">
+        <v>9757291</v>
+      </c>
+      <c r="C103" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B82" s="2">
-        <v>4444124</v>
-      </c>
-      <c r="C82" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B83" s="2">
-        <v>5006383</v>
-      </c>
-      <c r="C83" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B84" s="2">
-        <v>56869252</v>
-      </c>
-      <c r="C84" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B85" s="2">
-        <v>1823973</v>
-      </c>
-      <c r="C85" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B86" s="2">
-        <v>1257608</v>
-      </c>
-      <c r="C86" s="4">
-        <v>4550</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B87" s="2">
-        <v>9757291</v>
-      </c>
-      <c r="C87" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B88" s="2">
+      <c r="B104" s="2">
         <v>67424649</v>
       </c>
-      <c r="C88" s="4">
+      <c r="C104" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change bestClans and bestPlayers
</commit_message>
<xml_diff>
--- a/bestPlayers.xlsx
+++ b/bestPlayers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25121"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neo Dossier Alexis\Web Projects\BrawlhallaBestCountryPlayersRanksBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90F7D3B-8F28-4A9D-80EA-5D76463ECAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508A6245-8D93-4E46-9132-36462899CA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -513,8 +513,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}" name="France" displayName="France" ref="A1:D116" totalsRowShown="0">
   <autoFilter ref="A1:D116" xr:uid="{D12B8C86-4E93-4EAE-84B7-69A85E340F21}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D114">
-    <sortCondition ref="A1:A114"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D116">
+    <sortCondition ref="A1:A116"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D71A5C60-C9CB-4021-B21A-999D15C973E7}" name="Name" dataDxfId="2"/>
@@ -791,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
@@ -1973,10 +1973,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="B105" s="2">
-        <v>7808660</v>
+        <v>17545915</v>
       </c>
       <c r="C105" s="4">
         <v>0</v>
@@ -1984,10 +1984,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="B106" s="2">
-        <v>4444124</v>
+        <v>7808660</v>
       </c>
       <c r="C106" s="4">
         <v>0</v>
@@ -1995,10 +1995,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B107" s="2">
-        <v>5006383</v>
+        <v>4444124</v>
       </c>
       <c r="C107" s="4">
         <v>0</v>
@@ -2006,10 +2006,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="B108" s="2">
-        <v>1569376</v>
+        <v>5006383</v>
       </c>
       <c r="C108" s="4">
         <v>0</v>
@@ -2017,10 +2017,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="B109" s="2">
-        <v>56869252</v>
+        <v>1569376</v>
       </c>
       <c r="C109" s="4">
         <v>0</v>
@@ -2028,10 +2028,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B110" s="2">
-        <v>5034931</v>
+        <v>56869252</v>
       </c>
       <c r="C110" s="4">
         <v>0</v>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B111" s="2">
-        <v>1823973</v>
+        <v>5034931</v>
       </c>
       <c r="C111" s="4">
         <v>0</v>
@@ -2050,35 +2050,35 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B112" s="2">
-        <v>1257608</v>
+        <v>1823973</v>
       </c>
       <c r="C112" s="4">
-        <v>4550</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B113" s="2">
-        <v>9757291</v>
+        <v>1257608</v>
       </c>
       <c r="C113" s="4">
-        <v>0</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B114" s="2">
-        <v>67424649</v>
+        <v>9757291</v>
       </c>
       <c r="C114" s="4">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2094,13 +2094,13 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="B116" s="2">
-        <v>17545915</v>
+        <v>67424649</v>
       </c>
       <c r="C116" s="4">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>